<commit_message>
make data tables for LaTeX
</commit_message>
<xml_diff>
--- a/analysis/analysis copy.xlsx
+++ b/analysis/analysis copy.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Documents/School/2022/Methods/PSMT/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656649D7-F8DB-EF4B-8FC6-59F55A83B3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95AFD6D9-EFC1-C446-8851-07B170C5ADF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16920" yWindow="5540" windowWidth="26220" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13480" yWindow="29320" windowWidth="26220" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="points" sheetId="1" r:id="rId1"/>
     <sheet name="data for pgfplots" sheetId="2" r:id="rId2"/>
+    <sheet name="Data for pgfplots to cheat with" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>x</t>
   </si>
@@ -86,6 +87,36 @@
   </si>
   <si>
     <t>y8</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>R squared</t>
+  </si>
+  <si>
+    <t>f1</t>
+  </si>
+  <si>
+    <t>f2</t>
+  </si>
+  <si>
+    <t>f3</t>
+  </si>
+  <si>
+    <t>f4</t>
+  </si>
+  <si>
+    <t>f5</t>
+  </si>
+  <si>
+    <t>f6</t>
+  </si>
+  <si>
+    <t>f7</t>
+  </si>
+  <si>
+    <t>ffff8</t>
   </si>
 </sst>
 </file>
@@ -1273,7 +1304,7 @@
                   <c:y val="-0.13166145327983048"/>
                 </c:manualLayout>
               </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="0.00000" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -4764,7 +4795,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="0.00000" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -11511,7 +11542,7 @@
                   <c:y val="0.2516909776385407"/>
                 </c:manualLayout>
               </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="0.0000000000" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -13578,7 +13609,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="0.000000" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -14029,7 +14060,7 @@
                   <c:v>14.358161647039767</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>14.381933437846124</c:v>
+                  <c:v>14.381933437846101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14913,7 +14944,7 @@
                   <c:v>14.358161647039767</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>14.381933437846124</c:v>
+                  <c:v>14.381933437846101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15647,7 +15678,13 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="7.6049320945433443E-2"/>
+                  <c:y val="-6.0544467914633256E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="0.000000000000" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -16780,11 +16817,17 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="6"/>
+            <c:order val="3"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="8.0667060552913381E-2"/>
+                  <c:y val="0.18745715681399555"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="0.000000000000000" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -17363,7 +17406,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:numFmt formatCode="0.0000000000" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -18290,7 +18333,13 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.14392511361017826"/>
+                  <c:y val="-4.9828277525652796E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="0.0000000000" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -25090,10 +25139,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1263"/>
+  <dimension ref="A1:G1263"/>
   <sheetViews>
-    <sheetView topLeftCell="A913" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A925" sqref="A925:B1263"/>
+    <sheetView tabSelected="1" topLeftCell="C248" zoomScale="200" workbookViewId="0">
+      <selection activeCell="E259" sqref="E259:F263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27146,7 +27195,7 @@
         <v>67.655851727223066</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>6.0855784464274505</v>
       </c>
@@ -27154,7 +27203,7 @@
         <v>67.655851727223066</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>6.1093502372338078</v>
       </c>
@@ -27162,47 +27211,77 @@
         <v>67.655851727223066</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>6.133122028040165</v>
       </c>
       <c r="B259">
         <v>67.655851727223066</v>
       </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E259" t="s">
+        <v>0</v>
+      </c>
+      <c r="F259" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>6.1568938188465223</v>
       </c>
       <c r="B260">
         <v>67.655851727223066</v>
       </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E260">
+        <v>1</v>
+      </c>
+      <c r="F260">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>6.1806656096528796</v>
       </c>
       <c r="B261">
         <v>67.655851727223066</v>
       </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E261">
+        <v>9</v>
+      </c>
+      <c r="F261">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>6.2044374004592369</v>
       </c>
       <c r="B262">
         <v>67.809965284688275</v>
       </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E262">
+        <v>15</v>
+      </c>
+      <c r="F262">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>6.2282091912655941</v>
       </c>
       <c r="B263">
         <v>67.964078842153469</v>
       </c>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E263">
+        <v>19</v>
+      </c>
+      <c r="F263">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>6.2519809820719514</v>
       </c>
@@ -27210,7 +27289,7 @@
         <v>68.118192399618664</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>6.2757527728783087</v>
       </c>
@@ -27218,7 +27297,7 @@
         <v>68.118192399618664</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>6.299524563684666</v>
       </c>
@@ -27226,7 +27305,7 @@
         <v>68.272305957083873</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>6.3232963544910232</v>
       </c>
@@ -27234,7 +27313,7 @@
         <v>68.426419514549067</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>6.3470681452973805</v>
       </c>
@@ -27242,7 +27321,7 @@
         <v>68.426419514549067</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>6.3708399361037378</v>
       </c>
@@ -27250,7 +27329,7 @@
         <v>68.580533072014276</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>6.3946117269100951</v>
       </c>
@@ -27258,7 +27337,7 @@
         <v>68.734646629479471</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>6.4183835177164523</v>
       </c>
@@ -27266,7 +27345,7 @@
         <v>68.888760186944666</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>6.4421553085228087</v>
       </c>
@@ -27274,7 +27353,7 @@
         <v>69.042873744409874</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>6.465927099329166</v>
       </c>
@@ -27282,7 +27361,7 @@
         <v>69.042873744409874</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>6.4896988901355233</v>
       </c>
@@ -27290,7 +27369,7 @@
         <v>69.351100859340278</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>6.5134706809418805</v>
       </c>
@@ -27298,7 +27377,7 @@
         <v>69.505214416805472</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>6.5372424717482378</v>
       </c>
@@ -27306,7 +27385,7 @@
         <v>69.659327974270681</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>6.5610142625545951</v>
       </c>
@@ -27314,7 +27393,7 @@
         <v>69.813441531735876</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>6.5847860533609524</v>
       </c>
@@ -27322,7 +27401,7 @@
         <v>69.96755508920107</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>6.6085578441673096</v>
       </c>
@@ -27330,7 +27409,7 @@
         <v>69.96755508920107</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>6.6323296349736669</v>
       </c>
@@ -27338,7 +27417,7 @@
         <v>70.275782204131474</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>6.6561014257800242</v>
       </c>
@@ -27346,87 +27425,120 @@
         <v>70.429895761596683</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>6.6798732165863814</v>
       </c>
       <c r="B282">
         <v>70.738122876527086</v>
       </c>
-    </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F282" t="s">
+        <v>18</v>
+      </c>
+      <c r="G282" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>6.7036450073927387</v>
       </c>
       <c r="B283">
         <v>70.892236433992281</v>
       </c>
-    </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F283" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>6.727416798199096</v>
       </c>
       <c r="B284">
         <v>71.354577106387879</v>
       </c>
-    </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F284" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>6.7511885890054533</v>
       </c>
       <c r="B285">
         <v>71.816917778783477</v>
       </c>
-    </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F285" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>6.7749603798118105</v>
       </c>
       <c r="B286">
         <v>72.279258451179089</v>
       </c>
-    </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F286" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>6.7987321706181678</v>
       </c>
       <c r="B287">
         <v>72.587485566109493</v>
       </c>
-    </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F287" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>6.8225039614245251</v>
       </c>
       <c r="B288">
         <v>72.741599123574687</v>
       </c>
-    </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F288" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>6.8462757522308824</v>
       </c>
       <c r="B289">
         <v>72.895712681039882</v>
       </c>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F289" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A290">
         <v>6.8700475430372396</v>
       </c>
       <c r="B290">
         <v>73.203939795970285</v>
       </c>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F290" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A291">
         <v>6.8938193338435969</v>
       </c>
       <c r="B291">
         <v>73.358053353435494</v>
       </c>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F291" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>6.9175911246499533</v>
       </c>
@@ -27434,7 +27546,7 @@
         <v>73.666280468365898</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>6.9413629154563106</v>
       </c>
@@ -27442,7 +27554,7 @@
         <v>73.820394025831092</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>6.9651347062626678</v>
       </c>
@@ -27450,7 +27562,7 @@
         <v>74.28273469822669</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>6.9889064970690251</v>
       </c>
@@ -27458,7 +27570,7 @@
         <v>74.745075370622288</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>7.0126782878753824</v>
       </c>
@@ -27466,7 +27578,7 @@
         <v>75.053302485552692</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>7.0364500786817397</v>
       </c>
@@ -27474,7 +27586,7 @@
         <v>75.207416043017901</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>7.0602218694880969</v>
       </c>
@@ -27482,7 +27594,7 @@
         <v>75.361529600483095</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>7.0839936602944542</v>
       </c>
@@ -27490,7 +27602,7 @@
         <v>75.823870272878693</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>7.1077654511008115</v>
       </c>
@@ -27498,7 +27610,7 @@
         <v>76.286210945274306</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>7.1315372419071688</v>
       </c>
@@ -27506,7 +27618,7 @@
         <v>76.594438060204709</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>7.155309032713526</v>
       </c>
@@ -27514,7 +27626,7 @@
         <v>76.748551617669904</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A303">
         <v>7.1790808235198833</v>
       </c>
@@ -27522,7 +27634,7 @@
         <v>76.902665175135098</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A304">
         <v>7.2028526143262406</v>
       </c>
@@ -29940,7 +30052,7 @@
     </row>
     <row r="606" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A606">
-        <v>14.381933437846124</v>
+        <v>14.381933437846101</v>
       </c>
       <c r="B606">
         <v>115.12282742650486</v>
@@ -35212,8 +35324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A0076AD-3D82-654B-A4E1-25FFC8BDBDC9}">
   <dimension ref="A1:R1264"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D340"/>
+    <sheetView topLeftCell="B1" zoomScale="143" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -52962,4 +53074,1785 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251EC933-167B-474B-9CCF-5738A926DF84}">
+  <dimension ref="A1:F133"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>14.381933399999999</v>
+      </c>
+      <c r="B2">
+        <f>1.18946529*A2^6 - 110.37565129*A2^5 + 4255.22992131*A2^4 - 87229.99515716*A2^3 + 1002719.2417329*A2^2 - 6127618.75941031*A2 + 15550536.7216995</f>
+        <v>114.27623053826392</v>
+      </c>
+      <c r="C2">
+        <v>17.519809824285279</v>
+      </c>
+      <c r="D2">
+        <f>6046.77199932933*C2^6 - 651353.151682996*C2^5 + 29232785.7734147*C2^4 - 699672004.563012*C2^3 + 9419179590.35658*C2^2 - 67624182395.6474*C2 + 202279215616.422</f>
+        <v>133.1192626953125</v>
+      </c>
+      <c r="E2">
+        <v>18.423137874926852</v>
+      </c>
+      <c r="F2">
+        <f>3.4000047417*E2^3+199.6280602865*E2^2-3897.0360743426*E2+25388.8275429106</f>
+        <v>42609.701737869778</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>14.4057052</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B66" si="0">1.18946529*A3^6 - 110.37565129*A3^5 + 4255.22992131*A3^4 - 87229.99515716*A3^3 + 1002719.2417329*A3^2 - 6127618.75941031*A3 + 15550536.7216995</f>
+        <v>114.58605481125414</v>
+      </c>
+      <c r="C3">
+        <v>17.543581615091636</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D39" si="1">6046.77199932933*C3^6 - 651353.151682996*C3^5 + 29232785.7734147*C3^4 - 699672004.563012*C3^3 + 9419179590.35658*C3^2 - 67624182395.6474*C3 + 202279215616.422</f>
+        <v>132.5557861328125</v>
+      </c>
+      <c r="E3">
+        <v>18.446909665733209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>14.429477</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>114.83259847201407</v>
+      </c>
+      <c r="C4">
+        <v>17.567353405897993</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>132.6439208984375</v>
+      </c>
+      <c r="E4">
+        <v>18.470681456539566</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>14.453248800000001</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>115.01838492788374</v>
+      </c>
+      <c r="C5">
+        <v>17.59112519670435</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>133.0228271484375</v>
+      </c>
+      <c r="E5">
+        <v>18.494453247345923</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>14.477020599999999</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>115.14598941244185</v>
+      </c>
+      <c r="C6">
+        <v>17.614896987510708</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>133.4261474609375</v>
+      </c>
+      <c r="E6">
+        <v>18.518225038152281</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>14.5007924</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>115.21803269721568</v>
+      </c>
+      <c r="C7">
+        <v>17.638668778317065</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>133.6593017578125</v>
+      </c>
+      <c r="E7">
+        <v>18.541996828958638</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>14.5245642</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>115.23717443086207</v>
+      </c>
+      <c r="C8">
+        <v>17.662440569123422</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>133.5963134765625</v>
+      </c>
+      <c r="E8">
+        <v>18.565768619764995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>14.548336000000001</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>115.20610683597624</v>
+      </c>
+      <c r="C9">
+        <v>17.68621235992978</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>133.1646728515625</v>
+      </c>
+      <c r="E9">
+        <v>18.589540410571352</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>14.5721078</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>115.12754845060408</v>
+      </c>
+      <c r="C10">
+        <v>17.709984150736137</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>132.3363037109375</v>
+      </c>
+      <c r="E10">
+        <v>18.61331220137771</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>14.5958796</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>115.00423813797534</v>
+      </c>
+      <c r="C11">
+        <v>17.733755941542494</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>131.1182861328125</v>
+      </c>
+      <c r="E11">
+        <v>18.637083992184067</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>14.619651299999999</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>114.83893002010882</v>
+      </c>
+      <c r="C12">
+        <v>17.757527732348851</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>129.5435791015625</v>
+      </c>
+      <c r="E12">
+        <v>18.660855782990424</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>14.6434231</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>114.63438465632498</v>
+      </c>
+      <c r="C13">
+        <v>17.781299523155209</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>127.6671142578125</v>
+      </c>
+      <c r="E13">
+        <v>18.684627573796782</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>14.6671949</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>114.39336780644953</v>
+      </c>
+      <c r="C14">
+        <v>17.805071313961566</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>125.5523681640625</v>
+      </c>
+      <c r="E14">
+        <v>18.708399364603139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>14.690966700000001</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>114.11864223517478</v>
+      </c>
+      <c r="C15">
+        <v>17.828843104767923</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>123.2730712890625</v>
+      </c>
+      <c r="E15">
+        <v>18.732171155409496</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>14.714738499999999</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>113.81296310760081</v>
+      </c>
+      <c r="C16">
+        <v>17.85261489557428</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>120.9005126953125</v>
+      </c>
+      <c r="E16">
+        <v>18.755942946215853</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>14.7385103</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>113.47907322086394</v>
+      </c>
+      <c r="C17">
+        <v>17.876386686380638</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>118.5037841796875</v>
+      </c>
+      <c r="E17">
+        <v>18.779714737022211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>14.7622821</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>113.11969725228846</v>
+      </c>
+      <c r="C18">
+        <v>17.900158477186995</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>116.1448974609375</v>
+      </c>
+      <c r="E18">
+        <v>18.803486527828568</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>14.786053900000001</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>112.73753767646849</v>
+      </c>
+      <c r="C19">
+        <v>17.923930267993352</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>113.8753662109375</v>
+      </c>
+      <c r="E19">
+        <v>18.827258318634925</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>14.809825699999999</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>112.33526996709406</v>
+      </c>
+      <c r="C20">
+        <v>17.94770205879971</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>111.7337646484375</v>
+      </c>
+      <c r="E20">
+        <v>18.851030109441282</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>14.8335975</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>111.91553773917258</v>
+      </c>
+      <c r="C21">
+        <v>17.971473849606067</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>109.7457275390625</v>
+      </c>
+      <c r="E21">
+        <v>18.87480190024764</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>14.8573693</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>111.48094881512225</v>
+      </c>
+      <c r="C22">
+        <v>17.995245640412424</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>107.9227294921875</v>
+      </c>
+      <c r="E22">
+        <v>18.898573691053997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>14.881141</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>111.03407282568514</v>
+      </c>
+      <c r="C23">
+        <v>18.019017431218781</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>106.2618408203125</v>
+      </c>
+      <c r="E23">
+        <v>18.922345481860354</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>14.9049128</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>110.5774294976145</v>
+      </c>
+      <c r="C24">
+        <v>18.042789222025139</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>104.7474365234375</v>
+      </c>
+      <c r="E24">
+        <v>18.946117272666712</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>14.9286846</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>110.11349622346461</v>
+      </c>
+      <c r="C25">
+        <v>18.066561012831496</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>103.3514404296875</v>
+      </c>
+      <c r="E25">
+        <v>18.969889063473069</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>14.952456400000001</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>109.64469667710364</v>
+      </c>
+      <c r="C26">
+        <v>18.090332803637853</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>102.0382080078125</v>
+      </c>
+      <c r="E26">
+        <v>18.993660854279426</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>14.9762282</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>109.17339921928942</v>
+      </c>
+      <c r="C27">
+        <v>18.114104594444211</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>100.7655029296875</v>
+      </c>
+      <c r="E27">
+        <v>19.017432645085783</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>15</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>108.70191358961165</v>
+      </c>
+      <c r="C28">
+        <v>18.137876385250564</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>99.4925537109375</v>
+      </c>
+      <c r="E28">
+        <v>19.041204435892141</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>15.0237718</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>108.23248741962016</v>
+      </c>
+      <c r="C29">
+        <v>18.161648176056921</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>98.1778564453125</v>
+      </c>
+      <c r="E29">
+        <v>19.064976226698498</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>15.047543599999999</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>107.76730311848223</v>
+      </c>
+      <c r="C30">
+        <v>18.185419966863279</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>96.7935791015625</v>
+      </c>
+      <c r="E30">
+        <v>19.088748017504855</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>15.0713154</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>107.30847526527941</v>
+      </c>
+      <c r="C31">
+        <v>18.209191757669636</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>95.3248291015625</v>
+      </c>
+      <c r="E31">
+        <v>19.112519808311212</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>15.0950872</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>106.85804759897292</v>
+      </c>
+      <c r="C32">
+        <v>18.232963548475993</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>93.7813720703125</v>
+      </c>
+      <c r="E32">
+        <v>19.13629159911757</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>15.118859</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>106.41799000836909</v>
+      </c>
+      <c r="C33">
+        <v>18.256735339282351</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>92.2061767578125</v>
+      </c>
+      <c r="E33">
+        <v>19.160063389923927</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>15.1426307</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>105.99019869603217</v>
+      </c>
+      <c r="C34">
+        <v>18.280507130088708</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>90.6778564453125</v>
+      </c>
+      <c r="E34">
+        <v>19.183835180730284</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>15.1664025</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>105.57648556865752</v>
+      </c>
+      <c r="C35">
+        <v>18.304278920895065</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>89.3270263671875</v>
+      </c>
+      <c r="E35">
+        <v>19.207606971536642</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>15.190174300000001</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>105.17858801223338</v>
+      </c>
+      <c r="C36">
+        <v>18.328050711701422</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>88.3450927734375</v>
+      </c>
+      <c r="E36">
+        <v>19.231378762342999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>15.213946099999999</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>104.79815889336169</v>
+      </c>
+      <c r="C37">
+        <v>18.35182250250778</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="1"/>
+        <v>87.9925537109375</v>
+      </c>
+      <c r="E37">
+        <v>19.255150553149356</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>15.2377179</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>104.43676652945578</v>
+      </c>
+      <c r="C38">
+        <v>18.375594293314137</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="1"/>
+        <v>88.6173095703125</v>
+      </c>
+      <c r="E38">
+        <v>19.278922343955713</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>15.2614897</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>104.09589322842658</v>
+      </c>
+      <c r="C39">
+        <v>18.399366084120494</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>90.6593017578125</v>
+      </c>
+      <c r="E39">
+        <v>19.302694134762071</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>15.285261500000001</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>103.77693382836878</v>
+      </c>
+      <c r="E40">
+        <v>19.326465925568428</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>15.309033299999999</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>103.48119379021227</v>
+      </c>
+      <c r="E41">
+        <v>19.350237716374785</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>15.3328051</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>103.2098884973675</v>
+      </c>
+      <c r="E42">
+        <v>19.374009507181142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>15.3565769</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>102.96414189971983</v>
+      </c>
+      <c r="E43">
+        <v>19.3977812979875</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>15.380348700000001</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>102.74498550035059</v>
+      </c>
+      <c r="E44">
+        <v>19.421553088793857</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>15.4041204</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>102.55335843004286</v>
+      </c>
+      <c r="E45">
+        <v>19.445324879600214</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>15.4278922</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>102.39010364748538</v>
+      </c>
+      <c r="E46">
+        <v>19.469096670406572</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>15.451663999999999</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>102.25597252883017</v>
+      </c>
+      <c r="E47">
+        <v>19.492868461212929</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>15.4754358</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>102.15162087418139</v>
+      </c>
+      <c r="E48">
+        <v>19.516640252019286</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>15.4992076</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>102.0776097420603</v>
+      </c>
+      <c r="E49">
+        <v>19.540412042825643</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>15.522979400000001</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>102.03440537489951</v>
+      </c>
+      <c r="E50">
+        <v>19.564183833632001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>15.546751199999999</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>102.02237957157195</v>
+      </c>
+      <c r="E51">
+        <v>19.587955624438358</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>15.570523</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>102.04180974699557</v>
+      </c>
+      <c r="E52">
+        <v>19.611727415244715</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>15.5942948</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>102.09287928976119</v>
+      </c>
+      <c r="E53">
+        <v>19.635499206051072</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>15.618066600000001</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>102.17567866481841</v>
+      </c>
+      <c r="E54">
+        <v>19.65927099685743</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>15.641838399999999</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>102.2902055028826</v>
+      </c>
+      <c r="E55">
+        <v>19.683042787663787</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>15.6656101</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>102.43636518158019</v>
+      </c>
+      <c r="E56">
+        <v>19.706814578470144</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>15.689381900000001</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>102.6139746401459</v>
+      </c>
+      <c r="E57">
+        <v>19.730586369276502</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>15.713153699999999</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>102.82275974191725</v>
+      </c>
+      <c r="E58">
+        <v>19.754358160082859</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>15.7369255</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>103.0623588655144</v>
+      </c>
+      <c r="E59">
+        <v>19.778129950889216</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>15.7606973</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>103.33232393302023</v>
+      </c>
+      <c r="E60">
+        <v>19.801901741695573</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>15.784469100000001</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>103.63212222792208</v>
+      </c>
+      <c r="E61">
+        <v>19.825673532501931</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>15.808240899999999</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>103.96113830246031</v>
+      </c>
+      <c r="E62">
+        <v>19.849445323308288</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>15.8320127</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>104.31867558695376</v>
+      </c>
+      <c r="E63">
+        <v>19.873217114114645</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>15.8557845</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>104.70395895279944</v>
+      </c>
+      <c r="E64">
+        <v>19.896988904921002</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>15.879556300000001</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="0"/>
+        <v>105.11613685823977</v>
+      </c>
+      <c r="E65">
+        <v>19.92076069572736</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>15.903328</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="0"/>
+        <v>105.55428175069392</v>
+      </c>
+      <c r="E66">
+        <v>19.944532486533717</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>15.927099800000001</v>
+      </c>
+      <c r="B67">
+        <f t="shared" ref="B67:B130" si="2">1.18946529*A67^6 - 110.37565129*A67^5 + 4255.22992131*A67^4 - 87229.99515716*A67^3 + 1002719.2417329*A67^2 - 6127618.75941031*A67 + 15550536.7216995</f>
+        <v>106.01740037836134</v>
+      </c>
+      <c r="E67">
+        <v>19.968304277340074</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>15.950871599999999</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="2"/>
+        <v>106.50442563928664</v>
+      </c>
+      <c r="E68">
+        <v>19.992076068146432</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>15.9746434</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="2"/>
+        <v>107.01422628201544</v>
+      </c>
+      <c r="E69">
+        <v>20.015847858952789</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>15.9984152</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="2"/>
+        <v>107.54560858942568</v>
+      </c>
+      <c r="E70">
+        <v>20.039619649759143</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>16.022186999999999</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="2"/>
+        <v>108.0973194334656</v>
+      </c>
+      <c r="E71">
+        <v>20.0633914405655</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>16.045958800000001</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="2"/>
+        <v>108.66804988123477</v>
+      </c>
+      <c r="E72">
+        <v>20.087163231371857</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>16.0697306</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="2"/>
+        <v>109.25643836893141</v>
+      </c>
+      <c r="E73">
+        <v>20.110935022178214</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <v>16.093502399999998</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="2"/>
+        <v>109.86107476986945</v>
+      </c>
+      <c r="E74">
+        <v>20.134706812984572</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <v>16.117274200000001</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="2"/>
+        <v>110.48050397075713</v>
+      </c>
+      <c r="E75">
+        <v>20.158478603790929</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <v>16.141045999999999</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="2"/>
+        <v>111.11322985030711</v>
+      </c>
+      <c r="E76">
+        <v>20.182250394597286</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <v>16.1648177</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="2"/>
+        <v>111.75771738030016</v>
+      </c>
+      <c r="E77">
+        <v>20.206022185403643</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <v>16.188589499999999</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="2"/>
+        <v>112.41240648366511</v>
+      </c>
+      <c r="E78">
+        <v>20.229793976210001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>16.212361300000001</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="2"/>
+        <v>113.07570184208453</v>
+      </c>
+      <c r="E79">
+        <v>20.253565767016358</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>16.2361331</v>
+      </c>
+      <c r="B80">
+        <f t="shared" si="2"/>
+        <v>113.7459868285805</v>
+      </c>
+      <c r="E80">
+        <v>20.277337557822715</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>16.259904899999999</v>
+      </c>
+      <c r="B81">
+        <f t="shared" si="2"/>
+        <v>114.42162686027586</v>
+      </c>
+      <c r="E81">
+        <v>20.301109348629073</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>16.283676700000001</v>
+      </c>
+      <c r="B82">
+        <f t="shared" si="2"/>
+        <v>115.10097321309149</v>
+      </c>
+      <c r="E82">
+        <v>20.32488113943543</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>16.3074485</v>
+      </c>
+      <c r="B83">
+        <f t="shared" si="2"/>
+        <v>115.78236898221076</v>
+      </c>
+      <c r="E83">
+        <v>20.348652930241787</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <v>16.331220299999998</v>
+      </c>
+      <c r="B84">
+        <f t="shared" si="2"/>
+        <v>116.46415377594531</v>
+      </c>
+      <c r="E84">
+        <v>20.372424721048144</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <v>16.3549921</v>
+      </c>
+      <c r="B85">
+        <f t="shared" si="2"/>
+        <v>117.14466966129839</v>
+      </c>
+      <c r="E85">
+        <v>20.396196511854502</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <v>16.378763899999999</v>
+      </c>
+      <c r="B86">
+        <f t="shared" si="2"/>
+        <v>117.82226599194109</v>
+      </c>
+      <c r="E86">
+        <v>20.419968302660859</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <v>16.402535700000001</v>
+      </c>
+      <c r="B87">
+        <f t="shared" si="2"/>
+        <v>118.49530575610697</v>
+      </c>
+      <c r="E87">
+        <v>20.443740093467216</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>16.426307399999999</v>
+      </c>
+      <c r="B88">
+        <f t="shared" si="2"/>
+        <v>119.16216810978949</v>
+      </c>
+      <c r="E88">
+        <v>20.467511884273573</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>16.450079200000001</v>
+      </c>
+      <c r="B89">
+        <f t="shared" si="2"/>
+        <v>119.82126613892615</v>
+      </c>
+      <c r="E89">
+        <v>20.491283675079931</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>16.473851</v>
+      </c>
+      <c r="B90">
+        <f t="shared" si="2"/>
+        <v>120.47103565372527</v>
+      </c>
+      <c r="E90">
+        <v>20.515055465886288</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>16.497622799999998</v>
+      </c>
+      <c r="B91">
+        <f t="shared" si="2"/>
+        <v>121.10995332337916</v>
+      </c>
+      <c r="E91">
+        <v>20.538827256692645</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <v>16.521394600000001</v>
+      </c>
+      <c r="B92">
+        <f t="shared" si="2"/>
+        <v>121.73653961159289</v>
+      </c>
+      <c r="E92">
+        <v>20.562599047499003</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <v>16.545166399999999</v>
+      </c>
+      <c r="B93">
+        <f t="shared" si="2"/>
+        <v>122.34936619736254</v>
+      </c>
+      <c r="E93">
+        <v>20.58637083830536</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <v>16.568938200000002</v>
+      </c>
+      <c r="B94">
+        <f t="shared" si="2"/>
+        <v>122.94706208445132</v>
+      </c>
+      <c r="E94">
+        <v>20.610142629111717</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <v>16.59271</v>
+      </c>
+      <c r="B95">
+        <f t="shared" si="2"/>
+        <v>123.52832115627825</v>
+      </c>
+      <c r="E95">
+        <v>20.633914419918074</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <v>16.616481799999999</v>
+      </c>
+      <c r="B96">
+        <f t="shared" si="2"/>
+        <v>124.09190853871405</v>
+      </c>
+      <c r="E96">
+        <v>20.657686210724432</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>16.640253600000001</v>
+      </c>
+      <c r="B97">
+        <f t="shared" si="2"/>
+        <v>124.63666882552207</v>
+      </c>
+      <c r="E97">
+        <v>20.681458001530789</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <v>16.6640254</v>
+      </c>
+      <c r="B98">
+        <f t="shared" si="2"/>
+        <v>125.16153245605528</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>16.687797100000001</v>
+      </c>
+      <c r="B99">
+        <f t="shared" si="2"/>
+        <v>125.66552167572081</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>16.7115689</v>
+      </c>
+      <c r="B100">
+        <f t="shared" si="2"/>
+        <v>126.14776686765254</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <v>16.735340699999998</v>
+      </c>
+      <c r="B101">
+        <f t="shared" si="2"/>
+        <v>126.60750157572329</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
+        <v>16.759112500000001</v>
+      </c>
+      <c r="B102">
+        <f t="shared" si="2"/>
+        <v>127.04407859779894</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <v>16.782884299999999</v>
+      </c>
+      <c r="B103">
+        <f t="shared" si="2"/>
+        <v>127.45697637833655</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
+        <v>16.806656100000001</v>
+      </c>
+      <c r="B104">
+        <f t="shared" si="2"/>
+        <v>127.8458079341799</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
+        <v>16.8304279</v>
+      </c>
+      <c r="B105">
+        <f t="shared" si="2"/>
+        <v>128.21032800711691</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
+        <v>16.854199699999999</v>
+      </c>
+      <c r="B106">
+        <f t="shared" si="2"/>
+        <v>128.55044282414019</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <v>16.877971500000001</v>
+      </c>
+      <c r="B107">
+        <f t="shared" si="2"/>
+        <v>128.86621871031821</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
+        <v>16.9017433</v>
+      </c>
+      <c r="B108">
+        <f t="shared" si="2"/>
+        <v>129.15789035893977</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
+        <v>16.925515099999998</v>
+      </c>
+      <c r="B109">
+        <f t="shared" si="2"/>
+        <v>129.42587063647807</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
+        <v>16.949286799999999</v>
+      </c>
+      <c r="B110">
+        <f t="shared" si="2"/>
+        <v>129.67075894214213</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
+        <v>16.973058600000002</v>
+      </c>
+      <c r="B111">
+        <f t="shared" si="2"/>
+        <v>129.89335394836962</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
+        <v>16.9968304</v>
+      </c>
+      <c r="B112">
+        <f t="shared" si="2"/>
+        <v>130.09465735591948</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
+        <v>17.020602199999999</v>
+      </c>
+      <c r="B113">
+        <f t="shared" si="2"/>
+        <v>130.27588822878897</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="1">
+        <v>17.044374000000001</v>
+      </c>
+      <c r="B114">
+        <f t="shared" si="2"/>
+        <v>130.43849118985236</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="1">
+        <v>17.0681458</v>
+      </c>
+      <c r="B115">
+        <f t="shared" si="2"/>
+        <v>130.58414650894701</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="1">
+        <v>17.091917599999999</v>
+      </c>
+      <c r="B116">
+        <f t="shared" si="2"/>
+        <v>130.71478108502924</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="1">
+        <v>17.115689400000001</v>
+      </c>
+      <c r="B117">
+        <f t="shared" si="2"/>
+        <v>130.83257753588259</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="1">
+        <v>17.1394612</v>
+      </c>
+      <c r="B118">
+        <f t="shared" si="2"/>
+        <v>130.93998535908759</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="1">
+        <v>17.163233000000002</v>
+      </c>
+      <c r="B119">
+        <f t="shared" si="2"/>
+        <v>131.0397321972996</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="1">
+        <v>17.1870048</v>
+      </c>
+      <c r="B120">
+        <f t="shared" si="2"/>
+        <v>131.13483318127692</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="1">
+        <v>17.210776500000001</v>
+      </c>
+      <c r="B121">
+        <f t="shared" si="2"/>
+        <v>131.2286027316004</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="1">
+        <v>17.2345483</v>
+      </c>
+      <c r="B122">
+        <f t="shared" si="2"/>
+        <v>131.32466685213149</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="1">
+        <v>17.258320099999999</v>
+      </c>
+      <c r="B123">
+        <f t="shared" si="2"/>
+        <v>131.42697195149958</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="1">
+        <v>17.282091900000001</v>
+      </c>
+      <c r="B124">
+        <f t="shared" si="2"/>
+        <v>131.53979785181582</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="1">
+        <v>17.3058637</v>
+      </c>
+      <c r="B125">
+        <f t="shared" si="2"/>
+        <v>131.66776890493929</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="1">
+        <v>17.329635499999998</v>
+      </c>
+      <c r="B126">
+        <f t="shared" si="2"/>
+        <v>131.81586598791182</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="1">
+        <v>17.353407300000001</v>
+      </c>
+      <c r="B127">
+        <f t="shared" si="2"/>
+        <v>131.98943820036948</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="1">
+        <v>17.377179099999999</v>
+      </c>
+      <c r="B128">
+        <f t="shared" si="2"/>
+        <v>132.19421502389014</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="1">
+        <v>17.400950900000002</v>
+      </c>
+      <c r="B129">
+        <f t="shared" si="2"/>
+        <v>132.43631836213171</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="1">
+        <v>17.4247227</v>
+      </c>
+      <c r="B130">
+        <f t="shared" si="2"/>
+        <v>132.7222749684006</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="1">
+        <v>17.448494499999999</v>
+      </c>
+      <c r="B131">
+        <f t="shared" ref="B131:B133" si="3">1.18946529*A131^6 - 110.37565129*A131^5 + 4255.22992131*A131^4 - 87229.99515716*A131^3 + 1002719.2417329*A131^2 - 6127618.75941031*A131 + 15550536.7216995</f>
+        <v>133.05902878381312</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="1">
+        <v>17.4722662</v>
+      </c>
+      <c r="B132">
+        <f t="shared" si="3"/>
+        <v>133.4539521727711</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="1">
+        <v>17.496037999999999</v>
+      </c>
+      <c r="B133">
+        <f t="shared" si="3"/>
+        <v>133.91486530937254</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>